<commit_message>
Completed feature side on apollo website
</commit_message>
<xml_diff>
--- a/testsheet.xlsx
+++ b/testsheet.xlsx
@@ -525,12 +525,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Chief Technology Officer</t>
+          <t>Chief Financial Officer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Markus Ahlstrand</t>
+          <t>Carolina Walther</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>carolina@sesamy.com</t>
         </is>
       </c>
       <c r="E3" t="n">

</xml_diff>

<commit_message>
Made essential changes on the indeed side
</commit_message>
<xml_diff>
--- a/testsheet.xlsx
+++ b/testsheet.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,86 +477,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sesamy</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Chief Technology Officer</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Markus Ahlstrand</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>markus@sesamy.com</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Estimated $62.1K - $78.6K a year</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Does not have a source link on OpsWorks Co.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sesamy</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Chief Financial Officer</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Carolina Walther</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>carolina@sesamy.com</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Estimated $62.1K - $78.6K a year</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Does not have a source link on OpsWorks Co.</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>